<commit_message>
He hecho los tabpanes de datos en el que he añadido todo lo necesario para calcular la valoracion, he cambiado toda la interfaz y ademas he añadido graficos donus en los resultados que me dan
</commit_message>
<xml_diff>
--- a/informe_excel.xlsx
+++ b/informe_excel.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walth\Documents\NetBeansProjects\InterfazBaloncesto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3948123B-A195-4770-A67B-72535DC103F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F341742-EE2F-4EA8-A48C-70C4E5B58BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5256" yWindow="1212" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5172" yWindow="1644" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MiHoja" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="22">
   <si>
     <t>Nombre</t>
   </si>
@@ -34,13 +34,58 @@
     <t>TCI</t>
   </si>
   <si>
+    <t>TLI</t>
+  </si>
+  <si>
+    <t>Puntos</t>
+  </si>
+  <si>
     <t>%FG</t>
   </si>
   <si>
     <t>%eFG</t>
   </si>
   <si>
-    <t>Alvaro</t>
+    <t>%TS</t>
+  </si>
+  <si>
+    <t>Walther</t>
+  </si>
+  <si>
+    <t>promedios</t>
+  </si>
+  <si>
+    <t>Lebron</t>
+  </si>
+  <si>
+    <t>BRr</t>
+  </si>
+  <si>
+    <t>Wal</t>
+  </si>
+  <si>
+    <t>ewr</t>
+  </si>
+  <si>
+    <t>w234</t>
+  </si>
+  <si>
+    <t>etr</t>
+  </si>
+  <si>
+    <t>rte</t>
+  </si>
+  <si>
+    <t>Valoration</t>
+  </si>
+  <si>
+    <t>kyrdtf</t>
+  </si>
+  <si>
+    <t>tytyur</t>
+  </si>
+  <si>
+    <t>odknfsld</t>
   </si>
 </sst>
 </file>
@@ -393,15 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I4" sqref="A1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -419,29 +464,191 @@
       </c>
       <c r="F1" t="s" s="0">
         <v>5</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>3.0</v>
+        <v>78.0</v>
       </c>
       <c r="C2" t="n" s="0">
+        <v>33.0</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>610.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>223.0</v>
+      </c>
+      <c r="G2" t="n" s="0">
+        <v>12.79</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>15.49</v>
+      </c>
+      <c r="I2" t="n" s="0">
+        <v>17.7</v>
+      </c>
+      <c r="J2" t="n" s="0">
+        <v>-306.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>14.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>64.29</v>
+      </c>
+      <c r="I3" t="n" s="0">
+        <v>63.1</v>
+      </c>
+      <c r="J3" t="n" s="0">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="D2" t="n" s="0">
+      <c r="D4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
         <v>6.0</v>
       </c>
-      <c r="E2" t="n" s="0">
-        <v>50.0</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>58.33</v>
+      <c r="G4" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>125.0</v>
+      </c>
+      <c r="I4" t="n" s="0">
+        <v>104.17</v>
+      </c>
+      <c r="J4" t="n" s="0">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>130.0</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>65.0</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>205.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>379.0</v>
+      </c>
+      <c r="G5" t="n" s="0">
+        <v>63.41</v>
+      </c>
+      <c r="H5" t="n" s="0">
+        <v>79.27</v>
+      </c>
+      <c r="I5" t="n" s="0">
+        <v>76.1</v>
+      </c>
+      <c r="J5" t="n" s="0">
+        <v>194.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <f>AVERAGE(B2:B5)</f>
+        <v>54.25</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <f>AVERAGE(C2:C5)</f>
+        <v>25.75</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <f>AVERAGE(D2:D5)</f>
+        <v>207.75</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <f>AVERAGE(E2:E5)</f>
+        <v>38.25</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <f>AVERAGE(F2:F5)</f>
+        <v>157.25</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <f>AVERAGE(G2:G5)</f>
+        <v>56.55</v>
+      </c>
+      <c r="H6" t="n" s="0">
+        <f>AVERAGE(H2:H5)</f>
+        <v>71.0125</v>
+      </c>
+      <c r="I6" t="n" s="0">
+        <f>AVERAGE(I2:I5)</f>
+        <v>65.2675</v>
+      </c>
+      <c r="J6" t="n" s="0">
+        <f>AVERAGE(J2:J5)</f>
+        <v>-20.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
He añadido dos menus desplegables uno para el equipo y otro para el jugador. También he refactorizado toda la clase WritingExcel, y he añadido funcionalidades. He creado dos Excels y cada uno tiene sus datos
</commit_message>
<xml_diff>
--- a/informe_excel.xlsx
+++ b/informe_excel.xlsx
@@ -1,28 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walth\Documents\NetBeansProjects\InterfazBaloncesto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F341742-EE2F-4EA8-A48C-70C4E5B58BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B43BD42-0183-46AE-9DEC-4EF25E2B4F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5172" yWindow="1644" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="1320" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MiHoja" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="22">
-  <si>
-    <t>Nombre</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>Equipo</t>
+  </si>
+  <si>
+    <t>Jugador</t>
   </si>
   <si>
     <t>TCA</t>
@@ -49,43 +63,22 @@
     <t>%TS</t>
   </si>
   <si>
-    <t>Walther</t>
+    <t>Valoration</t>
+  </si>
+  <si>
+    <t>Angeles Lakers</t>
+  </si>
+  <si>
+    <t>Anthony Davis</t>
   </si>
   <si>
     <t>promedios</t>
   </si>
   <si>
-    <t>Lebron</t>
-  </si>
-  <si>
-    <t>BRr</t>
-  </si>
-  <si>
-    <t>Wal</t>
-  </si>
-  <si>
-    <t>ewr</t>
-  </si>
-  <si>
-    <t>w234</t>
-  </si>
-  <si>
-    <t>etr</t>
-  </si>
-  <si>
-    <t>rte</t>
-  </si>
-  <si>
-    <t>Valoration</t>
-  </si>
-  <si>
-    <t>kyrdtf</t>
-  </si>
-  <si>
-    <t>tytyur</t>
-  </si>
-  <si>
-    <t>odknfsld</t>
+    <t>Golden State Warriors</t>
+  </si>
+  <si>
+    <t>Klay Thompson</t>
   </si>
 </sst>
 </file>
@@ -438,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="A1:I4"/>
+      <selection activeCell="D4" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,176 +468,125 @@
         <v>8</v>
       </c>
       <c r="J1" t="s" s="0">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>78.0</v>
+        <v>11</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>12</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>33.0</v>
+        <v>4.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>610.0</v>
+        <v>2.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>45.0</v>
+        <v>6.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>223.0</v>
+        <v>2.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>12.79</v>
+        <v>12.0</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>15.49</v>
+        <v>66.67</v>
       </c>
       <c r="I2" t="n" s="0">
-        <v>17.7</v>
+        <v>83.33</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>-306.0</v>
+        <v>87.21</v>
+      </c>
+      <c r="K2" t="n" s="0">
+        <v>24.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>7.0</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>15</v>
       </c>
       <c r="C3" t="n" s="0">
         <v>4.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>14.0</v>
+        <v>2.0</v>
       </c>
       <c r="E3" t="n" s="0">
         <v>6.0</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>21.0</v>
+        <v>234.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>50.0</v>
+        <v>244.0</v>
       </c>
       <c r="H3" t="n" s="0">
-        <v>64.29</v>
+        <v>66.67</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>63.1</v>
+        <v>83.33</v>
       </c>
       <c r="J3" t="n" s="0">
-        <v>15.0</v>
+        <v>111.97</v>
+      </c>
+      <c r="K3" t="n" s="0">
+        <v>277.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B4" t="n" s="0">
+        <v>13</v>
+      </c>
+      <c r="B4" t="e" s="0">
+        <f>AVERAGE(B2:B3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <f>AVERAGE(C2:C3)</f>
+        <v>4.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <f>AVERAGE(D2:D3)</f>
         <v>2.0</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>2.0</v>
-      </c>
       <c r="E4" t="n" s="0">
-        <v>2.0</v>
+        <f>AVERAGE(E2:E3)</f>
+        <v>6.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>6.0</v>
+        <f>AVERAGE(F2:F3)</f>
+        <v>118.0</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>100.0</v>
+        <f>AVERAGE(G2:G3)</f>
+        <v>128.0</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>125.0</v>
+        <f>AVERAGE(H2:H3)</f>
+        <v>66.67</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>104.17</v>
+        <f>AVERAGE(I2:I3)</f>
+        <v>83.33</v>
       </c>
       <c r="J4" t="n" s="0">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>130.0</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>65.0</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>205.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>379.0</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>63.41</v>
-      </c>
-      <c r="H5" t="n" s="0">
-        <v>79.27</v>
-      </c>
-      <c r="I5" t="n" s="0">
-        <v>76.1</v>
-      </c>
-      <c r="J5" t="n" s="0">
-        <v>194.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B6" t="n" s="0">
-        <f>AVERAGE(B2:B5)</f>
-        <v>54.25</v>
-      </c>
-      <c r="C6" t="n" s="0">
-        <f>AVERAGE(C2:C5)</f>
-        <v>25.75</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <f>AVERAGE(D2:D5)</f>
-        <v>207.75</v>
-      </c>
-      <c r="E6" t="n" s="0">
-        <f>AVERAGE(E2:E5)</f>
-        <v>38.25</v>
-      </c>
-      <c r="F6" t="n" s="0">
-        <f>AVERAGE(F2:F5)</f>
-        <v>157.25</v>
-      </c>
-      <c r="G6" t="n" s="0">
-        <f>AVERAGE(G2:G5)</f>
-        <v>56.55</v>
-      </c>
-      <c r="H6" t="n" s="0">
-        <f>AVERAGE(H2:H5)</f>
-        <v>71.0125</v>
-      </c>
-      <c r="I6" t="n" s="0">
-        <f>AVERAGE(I2:I5)</f>
-        <v>65.2675</v>
-      </c>
-      <c r="J6" t="n" s="0">
-        <f>AVERAGE(J2:J5)</f>
-        <v>-20.5</v>
+        <f>AVERAGE(J2:J3)</f>
+        <v>99.59</v>
+      </c>
+      <c r="K4" t="n" s="0">
+        <f>AVERAGE(K2:K3)</f>
+        <v>150.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>